<commit_message>
https://github.com/jguiel/LIMS_Inventory_Management Added to inv.xlsx template added more barcodes and changed inv.xlsx to more clearly show the inv format with fake data
</commit_message>
<xml_diff>
--- a/input_inv/inv.xlsx
+++ b/input_inv/inv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfgui\Dropbox\Programming\Agena_Inv_GitHub\input_inv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63ECDF08-6E65-4BD9-A4F2-CB2F5BB21B44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E32F7D-7F28-42C7-A48B-C784E62A29CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{C0A0B0B2-2AE1-43FB-A1F6-1A7380DDFBC4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{C0A0B0B2-2AE1-43FB-A1F6-1A7380DDFBC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Lot</t>
   </si>
@@ -60,16 +60,145 @@
   </si>
   <si>
     <t>XE02933</t>
+  </si>
+  <si>
+    <t>XE02936</t>
+  </si>
+  <si>
+    <t>XE02937</t>
+  </si>
+  <si>
+    <t>XE02938</t>
+  </si>
+  <si>
+    <t>XE02939</t>
+  </si>
+  <si>
+    <t>XE02940</t>
+  </si>
+  <si>
+    <t>XE02941</t>
+  </si>
+  <si>
+    <t>XE02942</t>
+  </si>
+  <si>
+    <t>XE02943</t>
+  </si>
+  <si>
+    <t>XE30035</t>
+  </si>
+  <si>
+    <t>XE30036</t>
+  </si>
+  <si>
+    <t>XE30037</t>
+  </si>
+  <si>
+    <t>XE30038</t>
+  </si>
+  <si>
+    <t>XE30039</t>
+  </si>
+  <si>
+    <t>XE30040</t>
+  </si>
+  <si>
+    <t>XE30041</t>
+  </si>
+  <si>
+    <t>XE30042</t>
+  </si>
+  <si>
+    <t>XE30043</t>
+  </si>
+  <si>
+    <t>XE30044</t>
+  </si>
+  <si>
+    <t>XE30045</t>
+  </si>
+  <si>
+    <t>XE30046</t>
+  </si>
+  <si>
+    <t>XE30047</t>
+  </si>
+  <si>
+    <t>XE30048</t>
+  </si>
+  <si>
+    <t>XE67990</t>
+  </si>
+  <si>
+    <t>XE67991</t>
+  </si>
+  <si>
+    <t>XE67992</t>
+  </si>
+  <si>
+    <t>XE67993</t>
+  </si>
+  <si>
+    <t>XE67994</t>
+  </si>
+  <si>
+    <t>XE67995</t>
+  </si>
+  <si>
+    <t>XE67996</t>
+  </si>
+  <si>
+    <t>XE67997</t>
+  </si>
+  <si>
+    <t>XE67998</t>
+  </si>
+  <si>
+    <t>XE67999</t>
+  </si>
+  <si>
+    <t>XE68000</t>
+  </si>
+  <si>
+    <t>XE68001</t>
+  </si>
+  <si>
+    <t>XE68002</t>
+  </si>
+  <si>
+    <t>XE68003</t>
+  </si>
+  <si>
+    <t>XE68004</t>
+  </si>
+  <si>
+    <t>XE68005</t>
+  </si>
+  <si>
+    <t>XE68006</t>
+  </si>
+  <si>
+    <t>XE68007</t>
+  </si>
+  <si>
+    <t>XE68008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -411,18 +540,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5D944B-A58F-402F-865A-D38FB8E37C1B}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1234567</v>
       </c>
@@ -438,27 +567,118 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9A0C00D-0AD3-42E5-9AF3-C27A75290189}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>291746</v>
       </c>
@@ -474,27 +694,78 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B02F7B-9FEE-4139-A3CF-AC8DC4A0AB4F}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B3" sqref="B3:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>8273940</v>
       </c>
@@ -510,12 +781,78 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>